<commit_message>
Lean UX - Canvas adaptado
</commit_message>
<xml_diff>
--- a/Product Backlog.xlsx
+++ b/Product Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fmlima3\Desktop\Arte6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{50F23D19-4791-4271-B94F-195947FF57D2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA590AF-B1CB-49BA-8183-A82A20553450}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B4B6CA78-48C3-480B-9602-768895193B79}"/>
   </bookViews>
@@ -33,9 +33,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
-    <t>product Backlog</t>
-  </si>
-  <si>
     <t>id01</t>
   </si>
   <si>
@@ -64,6 +61,9 @@
   </si>
   <si>
     <t>Pesquisar contexto e nessecidades do negócio</t>
+  </si>
+  <si>
+    <t>product Backlog - sprint 1</t>
   </si>
 </sst>
 </file>
@@ -140,14 +140,14 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -663,7 +663,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,53 +673,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2"/>
+      <c r="A2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>6</v>
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>7</v>
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>9</v>
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>8</v>
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>10</v>
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>